<commit_message>
Added experimental code, changed threshold formula
</commit_message>
<xml_diff>
--- a/others/Threshold formula.xlsx
+++ b/others/Threshold formula.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Threshold</t>
   </si>
@@ -39,15 +39,56 @@
   <si>
     <t xml:space="preserve">Threshold at </t>
   </si>
+  <si>
+    <r>
+      <t>y = 0.00113159490529176x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 0.866937722472893x + 170.103701944699</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -106,11 +147,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -119,9 +166,6 @@
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -221,20 +265,6 @@
             <c:size val="7"/>
           </c:marker>
           <c:trendline>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.44688232720909887"/>
-                  <c:y val="2.178040244969379E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="0"/>
@@ -242,19 +272,19 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.43450817635245903"/>
-                  <c:y val="-2.5717045785943422E-2"/>
+                  <c:x val="0.46140690805938805"/>
+                  <c:y val="-2.4691236512102654E-2"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="#,##0.000000000000000000000000000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$17</c:f>
+              <c:f>Sheet1!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>144</c:v>
                 </c:pt>
@@ -296,60 +326,69 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$17</c:f>
+              <c:f>Sheet1!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>67.8</c:v>
+                  <c:v>71.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.400000000000006</c:v>
+                  <c:v>63.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59.4</c:v>
+                  <c:v>63.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61.2</c:v>
+                  <c:v>63.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.6</c:v>
+                  <c:v>29.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.400000000000006</c:v>
+                  <c:v>40.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.4</c:v>
+                  <c:v>26.950000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.200000000000003</c:v>
+                  <c:v>35.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.400000000000002</c:v>
+                  <c:v>26.45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.8</c:v>
+                  <c:v>16.649999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.8</c:v>
+                  <c:v>12.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.8</c:v>
+                  <c:v>12.15</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.8</c:v>
+                  <c:v>12.65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>7.8500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,10 +433,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$17</c:f>
+              <c:f>Sheet1!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>144</c:v>
                 </c:pt>
@@ -439,16 +478,22 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$17</c:f>
+              <c:f>Sheet1!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>114</c:v>
                 </c:pt>
@@ -492,7 +537,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -537,10 +585,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$17</c:f>
+              <c:f>Sheet1!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>144</c:v>
                 </c:pt>
@@ -582,16 +630,22 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$17</c:f>
+              <c:f>Sheet1!$F$3:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>37</c:v>
                 </c:pt>
@@ -635,7 +689,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,11 +707,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="79297152"/>
-        <c:axId val="117350784"/>
+        <c:axId val="66343680"/>
+        <c:axId val="66345216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79297152"/>
+        <c:axId val="66343680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,12 +721,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117350784"/>
+        <c:crossAx val="66345216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="117350784"/>
+        <c:axId val="66345216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,17 +737,424 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79297152"/>
+        <c:crossAx val="66343680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="3"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.69276016623955561"/>
+          <c:y val="0.1099595363079615"/>
+          <c:w val="0.29056247563781595"/>
+          <c:h val="0.50230314960629918"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wall diff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.43662461652472306"/>
+                  <c:y val="-0.10554607757363663"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>244</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No wall diff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.43662461652472306"/>
+                  <c:y val="-3.1219014289880432E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="67973504"/>
+        <c:axId val="67975040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="67973504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67975040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="67975040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67973504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -738,12 +1202,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>311394</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:G17" totalsRowShown="0">
-  <autoFilter ref="A2:G17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:G18" totalsRowShown="0">
+  <autoFilter ref="A2:G18"/>
   <sortState ref="A3:G16">
     <sortCondition ref="A3:A17"/>
   </sortState>
@@ -755,10 +1251,10 @@
     <tableColumn id="5" name="Wall diff" dataDxfId="2">
       <calculatedColumnFormula>B3-A3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="No wall diff" dataDxfId="0">
+    <tableColumn id="6" name="No wall diff" dataDxfId="1">
       <calculatedColumnFormula>D3-C3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Threshold" dataDxfId="1">
+    <tableColumn id="7" name="Threshold" dataDxfId="0">
       <calculatedColumnFormula>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1053,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1571,7 @@
         <v>7</v>
       </c>
       <c r="G1">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1115,16 +1611,16 @@
         <v>200</v>
       </c>
       <c r="E3" s="3">
-        <f>B3-A3</f>
+        <f t="shared" ref="E3:E17" si="0">B3-A3</f>
         <v>114</v>
       </c>
       <c r="F3" s="6">
-        <f>D3-C3</f>
+        <f t="shared" ref="F3:F17" si="1">D3-C3</f>
         <v>37</v>
       </c>
       <c r="G3">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>67.8</v>
+        <v>71.650000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1141,16 +1637,16 @@
         <v>200</v>
       </c>
       <c r="E4" s="4">
-        <f>B4-A4</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F4" s="7">
-        <f>D4-C4</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="G4" s="1">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>60.400000000000006</v>
+        <v>63.7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1167,16 +1663,16 @@
         <v>216</v>
       </c>
       <c r="E5" s="4">
-        <f>B5-A5</f>
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="F5" s="7">
-        <f>D5-C5</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="G5" s="1">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>59.4</v>
+        <v>63.45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1193,16 +1689,16 @@
         <v>191</v>
       </c>
       <c r="E6" s="3">
-        <f>B6-A6</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="F6" s="6">
-        <f>D6-C6</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="G6">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>61.2</v>
+        <v>63.35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1219,16 +1715,16 @@
         <v>277</v>
       </c>
       <c r="E7" s="3">
-        <f>B7-A7</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="F7" s="6">
-        <f>D7-C7</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G7">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>27.6</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1245,16 +1741,16 @@
         <v>245</v>
       </c>
       <c r="E8" s="3">
-        <f>B8-A8</f>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="F8" s="6">
-        <f>D8-C8</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="G8">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>38.400000000000006</v>
+        <v>40.700000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1271,16 +1767,16 @@
         <v>263</v>
       </c>
       <c r="E9" s="4">
-        <f>B9-A9</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="F9" s="7">
-        <f>D9-C9</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G9" s="1">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>25.4</v>
+        <v>26.950000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,16 +1793,16 @@
         <v>345</v>
       </c>
       <c r="E10" s="3">
-        <f>B10-A10</f>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="F10" s="6">
-        <f>D10-C10</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G10">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>32.200000000000003</v>
+        <v>35.6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1323,16 +1819,16 @@
         <v>300</v>
       </c>
       <c r="E11" s="3">
-        <f>B11-A11</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="F11" s="6">
-        <f>D11-C11</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G11">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>24.400000000000002</v>
+        <v>26.45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1349,16 +1845,16 @@
         <v>277</v>
       </c>
       <c r="E12" s="4">
-        <f>B12-A12</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F12" s="7">
-        <f>D12-C12</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G12" s="1">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>15.8</v>
+        <v>16.649999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1375,16 +1871,16 @@
         <v>274</v>
       </c>
       <c r="E13" s="4">
-        <f>B13-A13</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F13" s="7">
-        <f>D13-C13</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G13" s="1">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>11.8</v>
+        <v>12.15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1401,16 +1897,16 @@
         <v>278</v>
       </c>
       <c r="E14" s="3">
-        <f>B14-A14</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F14" s="6">
-        <f>D14-C14</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G14">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>11.8</v>
+        <v>12.15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1427,16 +1923,16 @@
         <v>337</v>
       </c>
       <c r="E15" s="3">
-        <f>B15-A15</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F15" s="6">
-        <f>D15-C15</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G15">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>11.8</v>
+        <v>12.65</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1453,34 +1949,93 @@
         <v>420</v>
       </c>
       <c r="E16" s="4">
-        <f>B16-A16</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F16" s="7">
-        <f>D16-C16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G16" s="1">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>306</v>
+      </c>
+      <c r="B17" s="2">
+        <v>321</v>
+      </c>
+      <c r="C17" s="5">
+        <v>343</v>
+      </c>
+      <c r="D17" s="5">
+        <v>345</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="1"/>
         <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4">
-        <f>B17-A17</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <f>D17-C17</f>
-        <v>0</v>
       </c>
       <c r="G17" s="1">
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
-        <v>0</v>
+        <v>7.8500000000000005</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>244</v>
+      </c>
+      <c r="B18" s="2">
+        <v>273</v>
+      </c>
+      <c r="C18" s="5">
+        <v>252</v>
+      </c>
+      <c r="D18" s="5">
+        <v>265</v>
+      </c>
+      <c r="E18" s="4">
+        <f>B18-A18</f>
+        <v>29</v>
+      </c>
+      <c r="F18" s="7">
+        <f>D18-C18</f>
+        <v>13</v>
+      </c>
+      <c r="G18" s="1">
+        <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
+        <v>20.2</v>
+      </c>
+      <c r="K18">
+        <v>1.13159490529176E-3</v>
+      </c>
+      <c r="L18">
+        <v>0.86693772247289302</v>
+      </c>
+      <c r="M18">
+        <v>170.103701944699</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>400</v>
+      </c>
+      <c r="J19">
+        <f>(0.0011*I19*I19)+(-0.8669*I19)+170.1</f>
+        <v>-0.65999999999999659</v>
+      </c>
+      <c r="K19">
+        <f>(K18*I19*I19)-(L18*I19)+M18</f>
+        <v>4.3837978022233983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Figured out the trendline issue, updated function
</commit_message>
<xml_diff>
--- a/others/Threshold formula.xlsx
+++ b/others/Threshold formula.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Threshold</t>
   </si>
@@ -65,12 +65,30 @@
       <t xml:space="preserve"> - 0.866937722472893x + 170.103701944699</t>
     </r>
   </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>=(([@[Wall diff]]-[@[No wall diff]])*$G$1)+[@[No wall diff]]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +111,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +164,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,11 +188,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -150,8 +222,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -707,11 +788,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66343680"/>
-        <c:axId val="66345216"/>
+        <c:axId val="45970560"/>
+        <c:axId val="45972096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66343680"/>
+        <c:axId val="45970560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -721,12 +802,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66345216"/>
+        <c:crossAx val="45972096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66345216"/>
+        <c:axId val="45972096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66343680"/>
+        <c:crossAx val="45970560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -822,16 +903,7 @@
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.43662461652472306"/>
-                  <c:y val="-0.10554607757363663"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -983,16 +1055,7 @@
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.43662461652472306"/>
-                  <c:y val="-3.1219014289880432E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1104,6 +1167,147 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threshold</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.47224368903161673"/>
+                  <c:y val="5.033209390492855E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00000000000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$20:$P$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$X$20:$X$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>67.865624723985178</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.8326928167711</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.64097357207902</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.290466989908921</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.781173070260806</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.11309181313468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.286223218530552</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.300567286448363</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.15612401688821</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.8528934098500214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.3908754653338029</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7700701833396058</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.9904775638673802</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0520976069171466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1118,44 +1322,100 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67973504"/>
-        <c:axId val="67975040"/>
+        <c:axId val="45823488"/>
+        <c:axId val="45825024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67973504"/>
+        <c:axId val="45823488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>LED off value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67975040"/>
+        <c:crossAx val="45825024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67975040"/>
+        <c:axId val="45825024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Difference between</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> LED on and off</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67973504"/>
+        <c:crossAx val="45823488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.69276016623955561"/>
+          <c:y val="5.4403980752405962E-2"/>
+          <c:w val="0.29056247563781595"/>
+          <c:h val="0.50230314960629918"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1549,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,7 +1826,7 @@
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1834,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>144</v>
       </c>
@@ -1623,7 +1883,7 @@
         <v>71.650000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>151</v>
       </c>
@@ -1649,7 +1909,7 @@
         <v>63.7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>159</v>
       </c>
@@ -1675,7 +1935,7 @@
         <v>63.45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>160</v>
       </c>
@@ -1701,7 +1961,7 @@
         <v>63.35</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>204</v>
       </c>
@@ -1726,8 +1986,11 @@
         <f>((Table2[[#This Row],[Wall diff]]-Table2[[#This Row],[No wall diff]])*$G$1)+Table2[[#This Row],[No wall diff]]</f>
         <v>29.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="X7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>212</v>
       </c>
@@ -1753,7 +2016,7 @@
         <v>40.700000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>216</v>
       </c>
@@ -1779,7 +2042,7 @@
         <v>26.950000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>237</v>
       </c>
@@ -1805,7 +2068,7 @@
         <v>35.6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>262</v>
       </c>
@@ -1831,7 +2094,7 @@
         <v>26.45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>267</v>
       </c>
@@ -1857,7 +2120,7 @@
         <v>16.649999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>299</v>
       </c>
@@ -1883,7 +2146,7 @@
         <v>12.15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>320</v>
       </c>
@@ -1909,7 +2172,7 @@
         <v>12.15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>338</v>
       </c>
@@ -1935,7 +2198,7 @@
         <v>12.65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>420</v>
       </c>
@@ -1961,7 +2224,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>306</v>
       </c>
@@ -1989,8 +2252,18 @@
       <c r="J17" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>244</v>
       </c>
@@ -2024,8 +2297,35 @@
       <c r="M18">
         <v>170.103701944699</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>12</v>
+      </c>
+      <c r="R18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" t="s">
+        <v>10</v>
+      </c>
+      <c r="T18" t="s">
+        <v>11</v>
+      </c>
+      <c r="U18" t="s">
+        <v>9</v>
+      </c>
+      <c r="V18" t="s">
+        <v>10</v>
+      </c>
+      <c r="W18" t="s">
+        <v>11</v>
+      </c>
+      <c r="X18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I19">
         <v>400</v>
       </c>
@@ -2037,8 +2337,271 @@
         <f>(K18*I19*I19)-(L18*I19)+M18</f>
         <v>4.3837978022233983</v>
       </c>
+      <c r="Q19" s="11">
+        <v>0.35</v>
+      </c>
+      <c r="R19">
+        <v>1.61603079270097E-3</v>
+      </c>
+      <c r="S19">
+        <v>-1.2764673500986199</v>
+      </c>
+      <c r="T19">
+        <v>258.75361398114399</v>
+      </c>
+      <c r="U19">
+        <v>7.4754623185714305E-4</v>
+      </c>
+      <c r="V19">
+        <v>-0.56975041734143295</v>
+      </c>
+      <c r="W19">
+        <v>109.363596510306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P20" s="12">
+        <v>140</v>
+      </c>
+      <c r="R20">
+        <f>(R$19*P20*P20)+(S$19*P20)+T$19</f>
+        <v>111.72238850427621</v>
+      </c>
+      <c r="U20">
+        <f>(U$19*P20*P20)+(V$19*P20)+W$19</f>
+        <v>44.250444226905387</v>
+      </c>
+      <c r="X20" s="10">
+        <f>((R20-U20)*Q$19)+U20</f>
+        <v>67.865624723985178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P21" s="12">
+        <v>160</v>
+      </c>
+      <c r="R21">
+        <f t="shared" ref="R21:R29" si="2">(R$19*P21*P21)+(S$19*P21)+T$19</f>
+        <v>95.889226258509638</v>
+      </c>
+      <c r="U21">
+        <f t="shared" ref="U21:U29" si="3">(U$19*P21*P21)+(V$19*P21)+W$19</f>
+        <v>37.340713271219585</v>
+      </c>
+      <c r="X21" s="10">
+        <f t="shared" ref="X21:X29" si="4">((R21-U21)*Q$19)+U21</f>
+        <v>57.8326928167711</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P22" s="12">
+        <v>180</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="2"/>
+        <v>81.348888646903845</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="3"/>
+        <v>31.029019301019503</v>
+      </c>
+      <c r="X22" s="10">
+        <f t="shared" si="4"/>
+        <v>48.64097357207902</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P23" s="12">
+        <v>200</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="2"/>
+        <v>68.101375669458832</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="3"/>
+        <v>25.315362316305126</v>
+      </c>
+      <c r="X23" s="10">
+        <f t="shared" si="4"/>
+        <v>40.290466989908921</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P24" s="12">
+        <v>220</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="2"/>
+        <v>56.146687326174572</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="3"/>
+        <v>20.19974231707647</v>
+      </c>
+      <c r="X24" s="10">
+        <f t="shared" si="4"/>
+        <v>32.781173070260806</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P25" s="12">
+        <v>240</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="2"/>
+        <v>45.484823617051092</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="3"/>
+        <v>15.682159303333535</v>
+      </c>
+      <c r="X25" s="10">
+        <f t="shared" si="4"/>
+        <v>26.11309181313468</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P26" s="12">
+        <v>260</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="2"/>
+        <v>36.11578454208842</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="3"/>
+        <v>11.762613275076319</v>
+      </c>
+      <c r="X26" s="10">
+        <f t="shared" si="4"/>
+        <v>20.286223218530552</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P27" s="12">
+        <v>280</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="2"/>
+        <v>28.039570101286444</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="3"/>
+        <v>8.4411042323047809</v>
+      </c>
+      <c r="X27" s="10">
+        <f t="shared" si="4"/>
+        <v>15.300567286448363</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P28" s="12">
+        <v>300</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="2"/>
+        <v>21.256180294645333</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="3"/>
+        <v>5.7176321750189913</v>
+      </c>
+      <c r="X28" s="10">
+        <f t="shared" si="4"/>
+        <v>11.15612401688821</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P29" s="12">
+        <v>320</v>
+      </c>
+      <c r="R29">
+        <f t="shared" ref="R29:R33" si="5">(R$19*P29*P29)+(S$19*P29)+T$19</f>
+        <v>15.765615122164974</v>
+      </c>
+      <c r="U29">
+        <f t="shared" ref="U29:U33" si="6">(U$19*P29*P29)+(V$19*P29)+W$19</f>
+        <v>3.5921971032188935</v>
+      </c>
+      <c r="X29" s="10">
+        <f t="shared" ref="X29:X33" si="7">((R29-U29)*Q$19)+U29</f>
+        <v>7.8528934098500214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P30" s="12">
+        <v>340</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="5"/>
+        <v>11.56787458384531</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="6"/>
+        <v>2.06479901690453</v>
+      </c>
+      <c r="X30" s="10">
+        <f t="shared" si="7"/>
+        <v>5.3908754653338029</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P31" s="12">
+        <v>360</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="5"/>
+        <v>8.6629586796865397</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="6"/>
+        <v>1.1354379160758725</v>
+      </c>
+      <c r="X31" s="10">
+        <f t="shared" si="7"/>
+        <v>3.7700701833396058</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P32" s="12">
+        <v>380</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="5"/>
+        <v>7.0508674096884931</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="6"/>
+        <v>0.80411380073293515</v>
+      </c>
+      <c r="X32" s="10">
+        <f t="shared" si="7"/>
+        <v>2.9904775638673802</v>
+      </c>
+    </row>
+    <row r="33" spans="16:24" x14ac:dyDescent="0.25">
+      <c r="P33" s="12">
+        <v>400</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="5"/>
+        <v>6.7316007738512553</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="6"/>
+        <v>1.0708266708757037</v>
+      </c>
+      <c r="X33" s="10">
+        <f t="shared" si="7"/>
+        <v>3.0520976069171466</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:W17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>